<commit_message>
Update test case status
</commit_message>
<xml_diff>
--- a/testing/ResortHub_TestCase.xlsx
+++ b/testing/ResortHub_TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leif.le\Documents\Leif\Work Space\ResortHub_Servlet\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6943ED2A-2D98-490C-AEED-4EAA86C5C640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E0E7F2D-7F5B-4A71-881F-F7709D0F9828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{923F7F89-0E2B-4835-A168-44C3E1B624BB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
   <si>
     <t>Case NO.</t>
   </si>
@@ -228,6 +228,15 @@
   </si>
   <si>
     <t>View booking details</t>
+  </si>
+  <si>
+    <t>Danh sách booking được hiển thị.</t>
+  </si>
+  <si>
+    <t>Recheck</t>
+  </si>
+  <si>
+    <t>Kiểm tra ngày đặt hợp lệ, role Admin dẫn tới trang Management</t>
   </si>
 </sst>
 </file>
@@ -371,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -447,6 +456,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -775,8 +787,8 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +799,7 @@
     <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.28515625" style="7" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="13"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
     <col min="8" max="8" width="36" style="7" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" style="18" customWidth="1"/>
     <col min="10" max="10" width="50" style="25" customWidth="1"/>
@@ -893,8 +905,8 @@
       <c r="H4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="19" t="s">
-        <v>55</v>
+      <c r="I4" s="29" t="s">
+        <v>65</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>60</v>
@@ -915,7 +927,9 @@
       <c r="F5" s="11"/>
       <c r="G5" s="3"/>
       <c r="H5" s="6"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="J5" s="6" t="s">
         <v>59</v>
       </c>
@@ -935,7 +949,9 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="6"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -975,8 +991,8 @@
       <c r="F8" s="11"/>
       <c r="G8" s="3"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="17" t="s">
-        <v>54</v>
+      <c r="I8" s="29" t="s">
+        <v>65</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>59</v>
@@ -995,7 +1011,9 @@
       <c r="F9" s="11"/>
       <c r="G9" s="3"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1033,7 +1051,9 @@
       <c r="F11" s="11"/>
       <c r="G11" s="3"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="J11" s="6" t="s">
         <v>59</v>
       </c>
@@ -1100,7 +1120,9 @@
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="I14" s="17" t="s">
         <v>54</v>
       </c>
@@ -1183,7 +1205,9 @@
       <c r="H18" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="I18" s="29" t="s">
+        <v>65</v>
+      </c>
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" ht="165" x14ac:dyDescent="0.25">
@@ -1203,8 +1227,8 @@
       <c r="H19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="19" t="s">
-        <v>55</v>
+      <c r="I19" s="29" t="s">
+        <v>65</v>
       </c>
       <c r="J19" s="6"/>
     </row>
@@ -1250,7 +1274,7 @@
       </c>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1265,10 +1289,12 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="9"/>
-      <c r="I22" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="J22" s="6"/>
+      <c r="I22" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
@@ -1285,8 +1311,8 @@
       <c r="F23" s="12"/>
       <c r="G23" s="1"/>
       <c r="H23" s="9"/>
-      <c r="I23" s="17" t="s">
-        <v>54</v>
+      <c r="I23" s="29" t="s">
+        <v>65</v>
       </c>
       <c r="J23" s="6"/>
     </row>

</xml_diff>